<commit_message>
Added new input jsons with nested approach
*Added new input jsons with nested approach
*WIP experiments in AnyLogic for dealing with the new inputs
</commit_message>
<xml_diff>
--- a/CaseDefinitions/industry_case/db_backboneConfig_industriecase.xlsx
+++ b/CaseDefinitions/industry_case/db_backboneConfig_industriecase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\cloudclient\run_cloud_experiments\input\industry_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\CaseDefinitions\industry_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9E68DA-FA88-412D-821A-0973AAF867B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF37D126-D538-42A4-AB31-293B3D601BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2490" windowWidth="26370" windowHeight="16995" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -271,6 +271,21 @@
   </si>
   <si>
     <t>a4</t>
+  </si>
+  <si>
+    <t>EHGV</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
   </si>
 </sst>
 </file>
@@ -719,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -817,7 +832,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1167,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1272,22 +1287,102 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>